<commit_message>
Add RoomInfo.cs, Add CardSubmitted(state processing) and PostProcessingQueue, Git Add .itemset in Debug folder
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\The Vampire Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire\TheVampire_Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8160" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="character ability" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -476,6 +476,10 @@
   </si>
   <si>
     <t>03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1038,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1182,6 +1186,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
       <c r="B8" s="6" t="s">
         <v>99</v>
       </c>
@@ -1275,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Modify PostProcessing, Add note at card model.xlsx
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -480,6 +480,10 @@
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31(은폐), 33(위장), 34(염탐)에 영향</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -840,7 +844,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1047,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1102,6 +1106,9 @@
       </c>
       <c r="G3" t="s">
         <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modify card model & message model (xlsx)
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -1047,7 +1047,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,7 @@
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="119.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.25" customWidth="1"/>
     <col min="8" max="8" width="53.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1290,7 +1290,7 @@
   <dimension ref="A2:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1303,7 +1303,7 @@
     <col min="6" max="6" width="14.25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="110.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="102.25" customWidth="1"/>
     <col min="10" max="10" width="48.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Add RoomInfoProcessing.cs, Add Processing(CardSubmit, Pre-PostProcessing), Modify card & message models
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire\TheVampire_Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\The Vampire Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,10 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 향한 모든 조사를 대상으로 조사자와 같은 팀으로 위장합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>대상의 정체를 파악합니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -108,10 +104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>모든 아군에게 자신의 정체를 알립니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>두 번 더 행동할 수 있습니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -364,10 +356,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>사격으로 공격받았을 경우 공격자의 정체를 파악합니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Effect Factor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -376,10 +364,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>저격 혹은 강타를 사용할 경우 두 번 공격합니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -484,6 +468,30 @@
   </si>
   <si>
     <t>31(은폐), 33(위장), 34(염탐)에 영향</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62(엄폐), 63(방어), 65(교란), 67(함정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62(엄폐), 63(방어), 65(교란), 66(반격), 67(함정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저격으로 공격받았을 경우 공격자의 정체를 파악합니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저격 혹은 강타를 사용할 경우 두배의 피해를 입힙니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군에게 자신의 정체를 알립니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조사자와 같은 팀으로 역할을 위장합니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -859,33 +867,33 @@
   <sheetData>
     <row r="2" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1">
         <v>0.05</v>
@@ -894,18 +902,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1">
         <v>0.1</v>
@@ -914,18 +922,18 @@
         <v>0.01</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
         <v>0.05</v>
@@ -934,18 +942,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
       </c>
       <c r="E6" s="1">
         <v>2.5000000000000001E-2</v>
@@ -954,18 +962,18 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>0.2</v>
@@ -974,18 +982,18 @@
         <v>0.01</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1">
         <v>0.2</v>
@@ -994,18 +1002,18 @@
         <v>0.01</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
@@ -1014,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -1047,7 +1055,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1063,10 +1071,10 @@
   <sheetData>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1084,18 +1092,18 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <f>(1 - SUM($E$5:$E$22)) / 2</f>
@@ -1105,21 +1113,21 @@
         <v>0.5</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1">
         <f>(1 - SUM($E$5:$E$22)) / 2</f>
@@ -1134,13 +1142,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>0.03</v>
@@ -1149,18 +1157,18 @@
         <v>0.5</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>0.03</v>
@@ -1169,12 +1177,12 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1189,21 +1197,21 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1">
         <v>0.03</v>
@@ -1212,18 +1220,18 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
       </c>
       <c r="E9" s="1">
         <v>0.03</v>
@@ -1232,18 +1240,18 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1">
         <v>0.03</v>
@@ -1252,21 +1260,21 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1">
         <v>0.03</v>
@@ -1275,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1298,7 @@
   <dimension ref="A2:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1299,20 +1307,20 @@
     <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.75" style="1" customWidth="1"/>
     <col min="9" max="9" width="102.25" customWidth="1"/>
-    <col min="10" max="10" width="48.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1321,10 +1329,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
@@ -1336,18 +1344,18 @@
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1">
         <v>6</v>
@@ -1363,18 +1371,21 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
@@ -1390,18 +1401,21 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
@@ -1411,18 +1425,18 @@
         <v>0.5</v>
       </c>
       <c r="I5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -1438,18 +1452,18 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
@@ -1464,18 +1478,18 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G8" s="1">
         <v>0.03</v>
@@ -1484,18 +1498,18 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
@@ -1510,18 +1524,18 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
@@ -1536,18 +1550,18 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G11" s="1">
         <v>0.03</v>
@@ -1556,18 +1570,18 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G12" s="1">
         <v>0.03</v>
@@ -1576,21 +1590,21 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1">
         <v>0.03</v>
@@ -1599,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify timer logic, Add turn processing
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -487,11 +487,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>조사자와 같은 팀으로 역할을 위장합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>아군에게 자신의 정체를 알립니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조사자와 같은 팀으로 역할을 위장합니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1055,7 +1055,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1157,7 +1157,7 @@
         <v>0.5</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modify .itemset, Fix item generation bug
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="character ability" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -568,6 +568,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,7 +855,7 @@
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B3" sqref="B3:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1052,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1106,8 +1109,8 @@
         <v>25</v>
       </c>
       <c r="E3" s="1">
-        <f>(1 - SUM($E$5:$E$22)) / 2</f>
-        <v>0.39500000000000002</v>
+        <f>(1 - SUM($E$5:$E$16)) / 2</f>
+        <v>0.35</v>
       </c>
       <c r="F3" s="1">
         <v>0.5</v>
@@ -1130,8 +1133,8 @@
         <v>26</v>
       </c>
       <c r="E4" s="1">
-        <f>(1 - SUM($E$5:$E$22)) / 2</f>
-        <v>0.39500000000000002</v>
+        <f>(1 - SUM($E$5:$E$16)) / 2</f>
+        <v>0.35</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -1151,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F5" s="1">
         <v>0.5</v>
@@ -1171,7 +1174,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -1191,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -1201,90 +1204,93 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>112</v>
-      </c>
       <c r="B8" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1">
         <v>0.03</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1297,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1365,7 +1371,7 @@
       </c>
       <c r="G3" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.19750000000000001</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -1395,7 +1401,7 @@
       </c>
       <c r="G4" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.19750000000000001</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -1419,7 +1425,7 @@
       </c>
       <c r="G5" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.19750000000000001</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="H5" s="1">
         <v>0.5</v>
@@ -1446,7 +1452,7 @@
       </c>
       <c r="G6" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.19750000000000001</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -1472,7 +1478,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
@@ -1492,7 +1498,7 @@
         <v>63</v>
       </c>
       <c r="G8" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -1518,7 +1524,7 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -1544,7 +1550,7 @@
         <v>0.2</v>
       </c>
       <c r="G10" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -1564,7 +1570,7 @@
         <v>47</v>
       </c>
       <c r="G11" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1584,7 +1590,7 @@
         <v>63</v>
       </c>
       <c r="G12" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
@@ -1607,7 +1613,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Test ver. (hp:10, itemsetVer:3(입막음,금제 제외))
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\The Vampire Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire\TheVampire_Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8160" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="character ability" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -568,9 +568,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1110,7 +1107,7 @@
       </c>
       <c r="E3" s="1">
         <f>(1 - SUM($E$5:$E$16)) / 2</f>
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="F3" s="1">
         <v>0.5</v>
@@ -1134,7 +1131,7 @@
       </c>
       <c r="E4" s="1">
         <f>(1 - SUM($E$5:$E$16)) / 2</f>
-        <v>0.35</v>
+        <v>0.375</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -1224,14 +1221,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1">
         <v>0.05</v>
@@ -1240,29 +1240,6 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1290,7 +1267,24 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1301,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J13"/>
+  <dimension ref="A2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1371,7 +1365,7 @@
       </c>
       <c r="G3" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -1401,7 +1395,7 @@
       </c>
       <c r="G4" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -1425,7 +1419,7 @@
       </c>
       <c r="G5" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H5" s="1">
         <v>0.5</v>
@@ -1452,7 +1446,7 @@
       </c>
       <c r="G6" s="1">
         <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -1580,14 +1574,17 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
       <c r="B12" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1">
         <v>0.05</v>
@@ -1596,30 +1593,27 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test ver. (hp:10), Fix dataStack bug, Modify itemset
</commit_message>
<xml_diff>
--- a/card model.xlsx
+++ b/card model.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,10 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 향한 모든 조사를 무효화합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>특별</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -64,10 +60,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대상의 정체를 파악합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>은폐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,10 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>두 번 더 행동할 수 있습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>도청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -200,18 +188,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 드러내지 않고 대상을 저격합니다\n피격자가 '파악'을 사용중일 경우 정체를 숨길 수 없습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>일반</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>근접하여 대상을 강하게 공격합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>빠른 몸놀림</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -244,10 +224,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 향한 모든 공격의 피해를 줄입니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>반격</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -256,10 +232,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 향한 모든 공격을 일정 확률로 회피합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>응급치료</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -308,14 +280,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 향한 공격 중 하나를 임의의 다른 사람에게 넘깁니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신을 향한 강타 공격 중 하나를 막고 반격합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>함정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,10 +288,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스스로 회복합니다\n함정에 의한 상처 또한 치료됩니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공통</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -352,18 +312,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대상이 조사를 성공할 경우 조사자와 피조사자의 정체를 파악합니다\n대상이 조사를 시도할 때 까지 효과가 사라지지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Effect Factor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신을 공격한 대상은 상처를 입고 지속적으로 피해를 입습니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -479,19 +431,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>저격으로 공격받았을 경우 공격자의 정체를 파악합니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>저격 혹은 강타를 사용할 경우 두배의 피해를 입힙니다\n사용하면 발동될 때 까지 효과가 사라지지 않습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조사자와 같은 팀으로 역할을 위장합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아군에게 자신의 정체를 알립니다</t>
+    <t>대상의 정체를 파악합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 향한 모든 조사를 무효화합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아군에게 자신의 정체를 알립니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조사자와 같은 팀으로 역할을 위장합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대상이 조사를 성공할 경우 조사자와 피조사자의 정체를 파악합니다.\n대상이 조사를 시도할 때 까지 효과가 사라지지 않습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저격으로 공격받았을 경우 공격자의 정체를 파악합니다.\n사용하면 발동될 때 까지 효과가 사라지지 않습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두 번 더 행동할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 드러내지 않고 대상을 저격합니다.\n피격자가 '파악'을 사용중일 경우 정체를 숨길 수 없습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근접하여 대상을 강하게 공격합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 향한 모든 공격을 일정 확률로 회피합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 향한 모든 공격의 피해를 줄입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스스로 회복합니다\n함정에 의한 상처 또한 치료됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 향한 공격 중 하나를 임의의 다른 사람에게 넘깁니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 향한 강타 공격 중 하나를 막고 반격합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신을 공격한 대상은 상처를 입고 지속적으로 피해를 입습니다.\n사용하면 발동될 때 까지 효과가 사라지지 않습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저격 혹은 강타를 사용할 경우 두배의 피해를 입힙니다.\n사용하면 발동될 때 까지 효과가 사라지지 않습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두 번 더 행동할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -547,7 +551,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -568,9 +572,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,33 +871,33 @@
   <sheetData>
     <row r="2" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <v>0.05</v>
@@ -905,18 +906,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1">
         <v>0.1</v>
@@ -925,18 +926,18 @@
         <v>0.01</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>0.05</v>
@@ -945,18 +946,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>2.5000000000000001E-2</v>
@@ -965,18 +966,18 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>0.2</v>
@@ -985,18 +986,18 @@
         <v>0.01</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1">
         <v>0.2</v>
@@ -1005,18 +1006,18 @@
         <v>0.01</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
@@ -1025,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -1055,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H18"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1074,10 +1075,10 @@
   <sheetData>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1086,72 +1087,72 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1">
-        <f>(1 - SUM($E$5:$E$16)) / 2</f>
-        <v>0.35</v>
+        <f>(1 - SUM($E$5:$E$15)) / 2</f>
+        <v>0.375</v>
       </c>
       <c r="F3" s="1">
         <v>0.5</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
-        <f>(1 - SUM($E$5:$E$16)) / 2</f>
-        <v>0.35</v>
+        <f>(1 - SUM($E$5:$E$15)) / 2</f>
+        <v>0.375</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>0.05</v>
@@ -1160,18 +1161,18 @@
         <v>0.5</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>0.05</v>
@@ -1180,18 +1181,18 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
         <v>0.05</v>
@@ -1200,18 +1201,18 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>0.05</v>
@@ -1220,18 +1221,21 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1">
         <v>0.05</v>
@@ -1240,57 +1244,51 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="1">
         <v>0.05</v>
       </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.03</v>
-      </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1301,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J13"/>
+  <dimension ref="A2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1323,10 +1321,10 @@
   <sheetData>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1335,33 +1333,33 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1">
         <v>6</v>
@@ -1370,28 +1368,28 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="1">
-        <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <f>(1 - SUM($G$7:$G$18)) / 4</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
@@ -1400,49 +1398,49 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="1">
-        <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <f>(1 - SUM($G$7:$G$18)) / 4</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1">
-        <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <f>(1 - SUM($G$7:$G$18)) / 4</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H5" s="1">
         <v>0.5</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -1451,25 +1449,25 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="1">
-        <f>(1 - SUM($G$7:$G$19)) / 4</f>
-        <v>0.16250000000000001</v>
+        <f>(1 - SUM($G$7:$G$18)) / 4</f>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
@@ -1484,18 +1482,18 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1">
         <v>0.05</v>
@@ -1504,18 +1502,18 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
@@ -1530,18 +1528,18 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
@@ -1556,18 +1554,18 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1">
         <v>0.05</v>
@@ -1576,18 +1574,21 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
       <c r="B12" s="6" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="G12" s="1">
         <v>0.05</v>
@@ -1596,30 +1597,27 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1">
         <v>0.05</v>
       </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>19</v>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>